<commit_message>
Updated scripts and knitted html versions of all Rmd files (closes #11)
</commit_message>
<xml_diff>
--- a/data/state-of-practice/data-extraction.xlsx
+++ b/data/state-of-practice/data-extraction.xlsx
@@ -14,53 +14,19 @@
   </sheets>
   <definedNames>
     <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Studies!$F$1:$F$137</definedName>
-    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Extraction!$U$3:$U$71</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">Extraction!$I$3:$J$70</definedName>
   </definedNames>
   <calcPr/>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision">
   <authors>
     <author/>
   </authors>
   <commentList>
-    <comment authorId="0" ref="M55">
-      <text>
-        <t xml:space="preserve">@davfuc@gmail.com I think this threat is rather "neglected": in the threats to conclusion validity, the authors claim that "We mitigated a threat of random heterogeneity of participants through two countermeasures: (i) we involved students so having samples of participates, in each experiment, with background and skills as much similar as possible; and (ii) the participants in each experiment underwent a training to make them as more homogeneous as possible within the groups." While this may be feasible, it still shows (1) that the authors were aware of the threat and (2) still did not model it in their analysis.
-_Assigned to davfuc@gmail.com_
-	-Julian Frattini
-Or is there any information I missed in the manuscript?
-	-Julian Frattini
-They acknowledge the threat and its importance and propose alternatives. In internal validity "This is why we suggested (in Section 5) conducting experiments with a 2 × 2 factorial design to better study the role that the experience with unit testing has in the relationship between TDD and the affective reactions of developers. " Where experience with unit testing is the relevant skill
-	-Davide Fucci
-But experience with unit testing is a different construct than individual skill. Experience with unit testing is a fixed (population-level) effect. The point of having a (G)LMM with a random effect is to model the individual performance of each participant (i.e., the random heterogeneity) without any inference of where this heterogeneity stems from.
-	-Julian Frattini
-yes. do we count this as a (failed) attempt at modeling random effect?
-	-Davide Fucci</t>
-      </text>
-    </comment>
-    <comment authorId="0" ref="M46">
-      <text>
-        <t xml:space="preserve">@davfuc@gmail.com I could not find evidence of modelling the subject-specific variance. Their GLMM seems to include several "Experience" factors, but these are on population level (i.e., fixed effects), not random effects explaining subject-specific variance.
-_Assigned to davfuc@gmail.com_
-	-Julian Frattini
-do we need to distinguish how skill is modeled rather than it is modeled? I agree that these measures of experience vary according to the individuals and should be random effect, so the authors model them wrongly (it seems, hard to say without the actual model formula)
-	-Davide Fucci
-The important factor is whether they model subject-specific variance (which is the purpose of a random effect in a GLMM). Experience is a population-level factor and, therefore, a different construct than individual skill. The Skill attribute receives the code "modeled" only if the (G)LMM contains a subject-specific random effect.
-	-Julian Frattini
-same as before. Do we see this as a failed attempt at modelling random effects?
-	-Davide Fucci</t>
-      </text>
-    </comment>
-    <comment authorId="0" ref="I67">
-      <text>
-        <t xml:space="preserve">LMM
-	-Davide Fucci</t>
-      </text>
-    </comment>
-    <comment authorId="0" ref="I62">
+    <comment authorId="0" ref="I66">
       <text>
         <t xml:space="preserve">LMM
 	-Davide Fucci</t>
@@ -84,7 +50,13 @@
 	-Davide Fucci</t>
       </text>
     </comment>
-    <comment authorId="0" ref="I55">
+    <comment authorId="0" ref="I58">
+      <text>
+        <t xml:space="preserve">LMM
+	-Davide Fucci</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="I54">
       <text>
         <t xml:space="preserve">LMM was applied to the overall analysis of the replications
 	-Davide Fucci</t>
@@ -125,7 +97,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1251" uniqueCount="396">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1241" uniqueCount="391">
   <si>
     <t>ID</t>
   </si>
@@ -719,6 +691,9 @@
     <t>questionnaire (pleasure, arousal, dominance); questionnaire (UEQ)</t>
   </si>
   <si>
+    <t>ANOVA-type Statistics</t>
+  </si>
+  <si>
     <t>The authors use a "ANOVA Type Statistic (ATS)" analysis method (section 4.7), which I am unfamiliar with - is this just "ANOVA"? Another paper (#49) claims that ATS is a non-parametric alternative to the ANOVA method. If so, how is it related to the Kruskal-Wallis test? Is a KW-test a type of ATS?</t>
   </si>
   <si>
@@ -827,6 +802,9 @@
     <t>We are not in agreement regarding the addressal of the "skill" threat yet (see comment on cell M46). Since skill represents a subject-specific variance that needs to be modeled with a random effect, it should not suffice to include an experience factor in the (G)LMM - as this would be a population-level effect.</t>
   </si>
   <si>
+    <t>I might have a third different view. To me, there is no evidence in the paper that they have incorporated the experience variables into the LMM. But they report the Kendall Tau. I vote for "isolated"?</t>
+  </si>
+  <si>
     <t>ways of operating on collection</t>
   </si>
   <si>
@@ -899,24 +877,6 @@
     <t>https://github.com/hassansartaj/aocl</t>
   </si>
   <si>
-    <t>language constructs</t>
-  </si>
-  <si>
-    <t>AIC;LE</t>
-  </si>
-  <si>
-    <t>code comprehension</t>
-  </si>
-  <si>
-    <t>#paremeters/#used_parameters;time</t>
-  </si>
-  <si>
-    <t>The authors apply an interesting N=1 design (https://en.wikipedia.org/wiki/N_of_1_trial). Can this be considered a crossover-design experiment?</t>
-  </si>
-  <si>
-    <t>These are trials performed on a single subject. So, they are not exactly crossover. I do not know how these experiments should be analyzed. The procedure for the regular crossover does not necessarily work here. I would not consider this as a crossover.</t>
-  </si>
-  <si>
     <t>TDD;non-TDD</t>
   </si>
   <si>
@@ -930,6 +890,9 @@
   </si>
   <si>
     <t>The authors talk about ANOVA-type statistics (ATS). For the addressal of the "skill" threat, we are not in agreement yet (see the comment on the "Skill" cell (M55).</t>
+  </si>
+  <si>
+    <t>There are several analyses in this paper and I think it is important to make explicit which is/are the ones we are focusing on. There is only one crossover out of the 3 experiments (Salerno). I understand we are focusing on this one only, aren´t we? Then there are the analyses corresponding to the aggregation of the 3 experiments conducted. But we are not focusing on these. So, I would say it is "neglected". They focus on the differences between participants during the aggregation of results only.</t>
   </si>
   <si>
     <t>Development approach;task</t>
@@ -1080,18 +1043,6 @@
     <t>SAM_questionnaire;UEQ_questionnaire</t>
   </si>
   <si>
-    <t>Subject- Number</t>
-  </si>
-  <si>
-    <t>Type</t>
-  </si>
-  <si>
-    <t>Availability</t>
-  </si>
-  <si>
-    <t>URL</t>
-  </si>
-  <si>
     <t>Representation format of business use cases</t>
   </si>
   <si>
@@ -1214,6 +1165,9 @@
     <t>Davide Fucci</t>
   </si>
   <si>
+    <t>Type</t>
+  </si>
+  <si>
     <t>Description</t>
   </si>
   <si>
@@ -1304,10 +1258,13 @@
     <t>Nonparametric test for related data points</t>
   </si>
   <si>
-    <t>Parametric test for unrelated data points of two or more samples</t>
-  </si>
-  <si>
-    <t>Nonparameteric test for unrelated data points of two or more samples</t>
+    <t>Parametric test for unrelated data points of three or more samples</t>
+  </si>
+  <si>
+    <t>Nonparametric test for unrelated data poitns of three or more samples</t>
+  </si>
+  <si>
+    <t>Nonparametric test for unrelated data points of three or more samples for a one-way layout</t>
   </si>
   <si>
     <t>In case none of the types fit</t>
@@ -1498,7 +1455,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="69">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -1591,9 +1548,6 @@
     <xf borderId="0" fillId="3" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="2" fillId="2" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="3" fillId="2" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="0" fillId="2" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" vertical="bottom"/>
     </xf>
@@ -3633,16 +3587,16 @@
         <v>Hanenberg, S., &amp; Mehlhorn, N. (2022). Two N-of-1 self-trials on readability differences between anonymous inner classes (AICs) and lambda expressions (LEs) on Java code snippets. Empirical Software Engineering, 27(2), 33.</v>
       </c>
       <c r="C48" s="7" t="b">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),TRUE)</f>
-        <v>1</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),FALSE)</f>
+        <v>0</v>
       </c>
       <c r="D48" s="8" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"dfu")</f>
         <v>dfu</v>
       </c>
-      <c r="E48" s="8">
+      <c r="E48" s="8" t="str">
         <f>IF(C48, COUNTIF(Extraction!A:A, A48), "-")</f>
-        <v>1</v>
+        <v>-</v>
       </c>
       <c r="F48" s="7" t="b">
         <f>IFERROR(__xludf.DUMMYFUNCTION("(COUNTIF(IMPORTRANGE(""https://docs.google.com/spreadsheets/d/1XUJGjtfB9SoW1rbohdkE9Z52MKac6AJzLHIsCSLTjGo/edit#gid=0"", ""Overlap!A2:A15""), A48)&gt;0)"),FALSE)</f>
@@ -6752,8 +6706,8 @@
     <col customWidth="1" min="3" max="5" width="25.13"/>
     <col customWidth="1" min="6" max="6" width="31.38"/>
     <col customWidth="1" min="7" max="7" width="8.25"/>
-    <col customWidth="1" min="8" max="8" width="16.38"/>
-    <col customWidth="1" min="10" max="10" width="20.13"/>
+    <col customWidth="1" min="8" max="8" width="17.25"/>
+    <col customWidth="1" min="10" max="10" width="22.5"/>
     <col customWidth="1" min="11" max="14" width="16.38"/>
     <col customWidth="1" min="15" max="15" width="10.13"/>
     <col customWidth="1" min="16" max="16" width="17.63"/>
@@ -8740,7 +8694,7 @@
         <v>91</v>
       </c>
       <c r="N33" s="5" t="s">
-        <v>91</v>
+        <v>47</v>
       </c>
       <c r="O33" s="19" t="b">
         <v>0</v>
@@ -8978,7 +8932,7 @@
         <v>45</v>
       </c>
       <c r="J37" s="23" t="s">
-        <v>183</v>
+        <v>194</v>
       </c>
       <c r="K37" s="5" t="s">
         <v>48</v>
@@ -9004,13 +8958,13 @@
       </c>
       <c r="S37" s="30"/>
       <c r="T37" s="20" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="U37" s="28" t="b">
         <v>1</v>
       </c>
       <c r="V37" s="20" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
     </row>
     <row r="38">
@@ -9022,16 +8976,16 @@
         <v>jfr</v>
       </c>
       <c r="C38" s="20" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="D38" s="21" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="E38" s="20" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="F38" s="22" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="G38" s="20">
         <v>24.0</v>
@@ -9081,22 +9035,22 @@
         <v>jfr</v>
       </c>
       <c r="C39" s="20" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="D39" s="21" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="E39" s="20" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="F39" s="22" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="G39" s="20">
         <v>8.0</v>
       </c>
       <c r="H39" s="19" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="I39" s="5" t="s">
         <v>69</v>
@@ -9140,22 +9094,22 @@
         <v>dfu</v>
       </c>
       <c r="C40" s="20" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="D40" s="21" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="E40" s="20" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="F40" s="22" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="G40" s="20">
         <v>59.0</v>
       </c>
       <c r="H40" s="19" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="I40" s="5" t="s">
         <v>69</v>
@@ -9199,22 +9153,22 @@
         <v>dfu</v>
       </c>
       <c r="C41" s="20" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="D41" s="21" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="E41" s="20" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="F41" s="22" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="G41" s="20">
         <v>79.0</v>
       </c>
       <c r="H41" s="19" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="I41" s="5" t="s">
         <v>69</v>
@@ -9258,16 +9212,16 @@
         <v>dfu</v>
       </c>
       <c r="C42" s="20" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="D42" s="21" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="E42" s="20" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="F42" s="22" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="G42" s="20">
         <v>17.0</v>
@@ -9319,16 +9273,16 @@
         <v>dfu</v>
       </c>
       <c r="C43" s="20" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="D43" s="21" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="E43" s="20" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="F43" s="22" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="G43" s="20">
         <v>15.0</v>
@@ -9359,13 +9313,13 @@
         <v>56</v>
       </c>
       <c r="Q43" s="26" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="R43" s="5" t="s">
         <v>56</v>
       </c>
       <c r="S43" s="27" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="T43" s="6"/>
       <c r="U43" s="25" t="b">
@@ -9382,16 +9336,16 @@
         <v>dfu</v>
       </c>
       <c r="C44" s="20" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="D44" s="21" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="E44" s="20" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="F44" s="22" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="G44" s="20">
         <v>31.0</v>
@@ -9441,16 +9395,16 @@
         <v>dfu</v>
       </c>
       <c r="C45" s="20" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="D45" s="21" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="E45" s="20" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="F45" s="22" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="G45" s="20">
         <v>48.0</v>
@@ -9481,13 +9435,13 @@
         <v>56</v>
       </c>
       <c r="Q45" s="26" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="R45" s="5" t="s">
         <v>56</v>
       </c>
       <c r="S45" s="27" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="T45" s="6"/>
       <c r="U45" s="25" t="b">
@@ -9504,16 +9458,16 @@
         <v>dfu</v>
       </c>
       <c r="C46" s="20" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="D46" s="21" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="E46" s="20" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="F46" s="22" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="G46" s="20">
         <v>32.0</v>
@@ -9532,7 +9486,7 @@
         <v>47</v>
       </c>
       <c r="M46" s="5" t="s">
-        <v>91</v>
+        <v>64</v>
       </c>
       <c r="N46" s="5" t="s">
         <v>47</v>
@@ -9544,21 +9498,23 @@
         <v>56</v>
       </c>
       <c r="Q46" s="26" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="R46" s="5" t="s">
         <v>56</v>
       </c>
       <c r="S46" s="27" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="T46" s="20" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="U46" s="28" t="b">
         <v>1</v>
       </c>
-      <c r="V46" s="6"/>
+      <c r="V46" s="20" t="s">
+        <v>231</v>
+      </c>
     </row>
     <row r="47">
       <c r="A47" s="5">
@@ -9569,16 +9525,16 @@
         <v>dfu</v>
       </c>
       <c r="C47" s="20" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="D47" s="21" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="E47" s="20" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="F47" s="22" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="G47" s="20">
         <v>20.0</v>
@@ -9615,7 +9571,7 @@
         <v>188</v>
       </c>
       <c r="S47" s="32" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="T47" s="6"/>
       <c r="U47" s="25" t="b">
@@ -9632,16 +9588,16 @@
         <v>dfu</v>
       </c>
       <c r="C48" s="20" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="D48" s="21" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="E48" s="20" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="F48" s="22" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="G48" s="20">
         <v>45.0</v>
@@ -9672,13 +9628,13 @@
         <v>56</v>
       </c>
       <c r="Q48" s="26" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="R48" s="5" t="s">
         <v>56</v>
       </c>
       <c r="S48" s="27" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="T48" s="6"/>
       <c r="U48" s="25" t="b">
@@ -9695,16 +9651,16 @@
         <v>dfu</v>
       </c>
       <c r="C49" s="20" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="D49" s="21" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="E49" s="20" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="F49" s="22" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="G49" s="20">
         <v>27.0</v>
@@ -9735,13 +9691,13 @@
         <v>56</v>
       </c>
       <c r="Q49" s="26" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="R49" s="5" t="s">
         <v>56</v>
       </c>
       <c r="S49" s="27" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="T49" s="6"/>
       <c r="U49" s="25" t="b">
@@ -9758,16 +9714,16 @@
         <v>dfu</v>
       </c>
       <c r="C50" s="20" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="D50" s="21" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="E50" s="20" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="F50" s="22" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="G50" s="20">
         <v>24.0</v>
@@ -9798,13 +9754,13 @@
         <v>56</v>
       </c>
       <c r="Q50" s="26" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="R50" s="5" t="s">
         <v>56</v>
       </c>
       <c r="S50" s="27" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="T50" s="6"/>
       <c r="U50" s="25" t="b">
@@ -9821,16 +9777,16 @@
         <v>dfu</v>
       </c>
       <c r="C51" s="20" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="D51" s="21" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="E51" s="20" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="F51" s="22" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="G51" s="20">
         <v>40.0</v>
@@ -9863,7 +9819,7 @@
         <v>188</v>
       </c>
       <c r="Q51" s="31" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="R51" s="5" t="s">
         <v>49</v>
@@ -9884,16 +9840,16 @@
         <v>dfu</v>
       </c>
       <c r="C52" s="20" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="D52" s="21" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="E52" s="20" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="F52" s="22" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="G52" s="20">
         <v>55.0</v>
@@ -9945,16 +9901,16 @@
         <v>dfu</v>
       </c>
       <c r="C53" s="20" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="D53" s="5" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="E53" s="21" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="F53" s="22" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="G53" s="20">
         <v>124.0</v>
@@ -9987,7 +9943,7 @@
         <v>188</v>
       </c>
       <c r="Q53" s="26" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="R53" s="5" t="s">
         <v>49</v>
@@ -10001,101 +9957,101 @@
     </row>
     <row r="54">
       <c r="A54" s="5">
-        <v>47.0</v>
+        <v>49.0</v>
       </c>
       <c r="B54" s="19" t="str">
         <f>IF(ISBLANK(A54), "", VLOOKUP(A54, Studies!A:D, 4))</f>
         <v>dfu</v>
       </c>
       <c r="C54" s="20" t="s">
-        <v>254</v>
+        <v>132</v>
       </c>
       <c r="D54" s="21" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="E54" s="20" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="F54" s="22" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="G54" s="20">
-        <v>8.0</v>
+        <v>29.0</v>
       </c>
       <c r="H54" s="19" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="I54" s="5" t="s">
         <v>45</v>
       </c>
       <c r="J54" s="23" t="s">
-        <v>183</v>
+        <v>194</v>
       </c>
       <c r="K54" s="5" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="L54" s="5" t="s">
-        <v>64</v>
+        <v>48</v>
       </c>
       <c r="M54" s="5" t="s">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="N54" s="5" t="s">
         <v>64</v>
       </c>
       <c r="O54" s="19" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P54" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="Q54" s="29"/>
+        <v>56</v>
+      </c>
+      <c r="Q54" s="26" t="s">
+        <v>259</v>
+      </c>
       <c r="R54" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="S54" s="30"/>
+        <v>56</v>
+      </c>
+      <c r="S54" s="32" t="s">
+        <v>259</v>
+      </c>
       <c r="T54" s="20" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="U54" s="28" t="b">
         <v>1</v>
       </c>
       <c r="V54" s="20" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="5">
-        <v>49.0</v>
+        <v>53.0</v>
       </c>
       <c r="B55" s="19" t="str">
         <f>IF(ISBLANK(A55), "", VLOOKUP(A55, Studies!A:D, 4))</f>
         <v>dfu</v>
       </c>
       <c r="C55" s="20" t="s">
-        <v>132</v>
+        <v>262</v>
       </c>
       <c r="D55" s="21" t="s">
-        <v>260</v>
+        <v>263</v>
       </c>
       <c r="E55" s="20" t="s">
-        <v>261</v>
+        <v>264</v>
       </c>
       <c r="F55" s="22" t="s">
-        <v>262</v>
-      </c>
-      <c r="G55" s="20">
-        <v>29.0</v>
-      </c>
+        <v>265</v>
+      </c>
+      <c r="G55" s="20"/>
       <c r="H55" s="19" t="s">
-        <v>44</v>
+        <v>126</v>
       </c>
       <c r="I55" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="J55" s="23" t="s">
-        <v>183</v>
-      </c>
+        <v>69</v>
+      </c>
+      <c r="J55" s="24"/>
       <c r="K55" s="5" t="s">
         <v>48</v>
       </c>
@@ -10106,64 +10062,64 @@
         <v>47</v>
       </c>
       <c r="N55" s="5" t="s">
-        <v>64</v>
+        <v>47</v>
       </c>
       <c r="O55" s="19" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P55" s="5" t="s">
         <v>56</v>
       </c>
       <c r="Q55" s="26" t="s">
-        <v>263</v>
+        <v>266</v>
       </c>
       <c r="R55" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="S55" s="32" t="s">
-        <v>263</v>
-      </c>
-      <c r="T55" s="20" t="s">
-        <v>264</v>
-      </c>
-      <c r="U55" s="28" t="b">
-        <v>1</v>
+      <c r="S55" s="27" t="s">
+        <v>266</v>
+      </c>
+      <c r="T55" s="6"/>
+      <c r="U55" s="25" t="b">
+        <v>0</v>
       </c>
       <c r="V55" s="6"/>
     </row>
     <row r="56">
       <c r="A56" s="5">
-        <v>53.0</v>
+        <v>55.0</v>
       </c>
       <c r="B56" s="19" t="str">
         <f>IF(ISBLANK(A56), "", VLOOKUP(A56, Studies!A:D, 4))</f>
         <v>dfu</v>
       </c>
       <c r="C56" s="20" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
       <c r="D56" s="21" t="s">
-        <v>266</v>
+        <v>268</v>
       </c>
       <c r="E56" s="20" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="F56" s="22" t="s">
-        <v>268</v>
-      </c>
-      <c r="G56" s="20"/>
+        <v>270</v>
+      </c>
+      <c r="G56" s="20">
+        <v>144.0</v>
+      </c>
       <c r="H56" s="19" t="s">
-        <v>126</v>
+        <v>44</v>
       </c>
       <c r="I56" s="5" t="s">
         <v>69</v>
       </c>
       <c r="J56" s="24"/>
       <c r="K56" s="5" t="s">
-        <v>48</v>
+        <v>91</v>
       </c>
       <c r="L56" s="5" t="s">
-        <v>48</v>
+        <v>91</v>
       </c>
       <c r="M56" s="5" t="s">
         <v>47</v>
@@ -10178,15 +10134,17 @@
         <v>56</v>
       </c>
       <c r="Q56" s="26" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
       <c r="R56" s="5" t="s">
         <v>56</v>
       </c>
       <c r="S56" s="27" t="s">
-        <v>269</v>
-      </c>
-      <c r="T56" s="6"/>
+        <v>271</v>
+      </c>
+      <c r="T56" s="20" t="s">
+        <v>272</v>
+      </c>
       <c r="U56" s="25" t="b">
         <v>0</v>
       </c>
@@ -10194,36 +10152,37 @@
     </row>
     <row r="57">
       <c r="A57" s="5">
-        <v>55.0</v>
-      </c>
-      <c r="B57" s="19" t="str">
-        <f>IF(ISBLANK(A57), "", VLOOKUP(A57, Studies!A:D, 4))</f>
-        <v>dfu</v>
+        <v>57.0</v>
+      </c>
+      <c r="B57" s="19" t="s">
+        <v>273</v>
       </c>
       <c r="C57" s="20" t="s">
-        <v>270</v>
+        <v>274</v>
       </c>
       <c r="D57" s="21" t="s">
-        <v>271</v>
+        <v>275</v>
       </c>
       <c r="E57" s="20" t="s">
-        <v>272</v>
+        <v>276</v>
       </c>
       <c r="F57" s="22" t="s">
-        <v>273</v>
+        <v>277</v>
       </c>
       <c r="G57" s="20">
-        <v>144.0</v>
+        <v>20.0</v>
       </c>
       <c r="H57" s="19" t="s">
-        <v>44</v>
+        <v>126</v>
       </c>
       <c r="I57" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="J57" s="24"/>
+        <v>45</v>
+      </c>
+      <c r="J57" s="23" t="s">
+        <v>183</v>
+      </c>
       <c r="K57" s="5" t="s">
-        <v>91</v>
+        <v>48</v>
       </c>
       <c r="L57" s="5" t="s">
         <v>91</v>
@@ -10232,26 +10191,22 @@
         <v>47</v>
       </c>
       <c r="N57" s="5" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="O57" s="19" t="b">
         <v>0</v>
       </c>
       <c r="P57" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="Q57" s="26" t="s">
-        <v>274</v>
+        <v>83</v>
+      </c>
+      <c r="Q57" s="31" t="s">
+        <v>278</v>
       </c>
       <c r="R57" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="S57" s="27" t="s">
-        <v>274</v>
-      </c>
-      <c r="T57" s="20" t="s">
-        <v>275</v>
-      </c>
+        <v>49</v>
+      </c>
+      <c r="S57" s="30"/>
+      <c r="T57" s="6"/>
       <c r="U57" s="25" t="b">
         <v>0</v>
       </c>
@@ -10259,60 +10214,61 @@
     </row>
     <row r="58">
       <c r="A58" s="5">
-        <v>57.0</v>
-      </c>
-      <c r="B58" s="19" t="s">
-        <v>276</v>
+        <v>60.0</v>
+      </c>
+      <c r="B58" s="19" t="str">
+        <f>IF(ISBLANK(A58), "", VLOOKUP(A58, Studies!A:D, 4))</f>
+        <v>dfu</v>
       </c>
       <c r="C58" s="20" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="D58" s="21" t="s">
-        <v>278</v>
+        <v>238</v>
       </c>
       <c r="E58" s="20" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="F58" s="22" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="G58" s="20">
-        <v>20.0</v>
+        <v>18.0</v>
       </c>
       <c r="H58" s="19" t="s">
-        <v>126</v>
+        <v>90</v>
       </c>
       <c r="I58" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="J58" s="23" t="s">
-        <v>183</v>
-      </c>
+        <v>69</v>
+      </c>
+      <c r="J58" s="24"/>
       <c r="K58" s="5" t="s">
-        <v>48</v>
+        <v>91</v>
       </c>
       <c r="L58" s="5" t="s">
         <v>91</v>
       </c>
       <c r="M58" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="N58" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="N58" s="5" t="s">
-        <v>48</v>
-      </c>
       <c r="O58" s="19" t="b">
         <v>0</v>
       </c>
       <c r="P58" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="Q58" s="31" t="s">
-        <v>281</v>
+        <v>56</v>
+      </c>
+      <c r="Q58" s="26" t="s">
+        <v>282</v>
       </c>
       <c r="R58" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="S58" s="30"/>
+        <v>56</v>
+      </c>
+      <c r="S58" s="27" t="s">
+        <v>282</v>
+      </c>
       <c r="T58" s="6"/>
       <c r="U58" s="25" t="b">
         <v>0</v>
@@ -10328,19 +10284,19 @@
         <v>dfu</v>
       </c>
       <c r="C59" s="20" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="D59" s="21" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="E59" s="20" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="F59" s="22" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="G59" s="20">
-        <v>18.0</v>
+        <v>10.0</v>
       </c>
       <c r="H59" s="19" t="s">
         <v>90</v>
@@ -10368,13 +10324,13 @@
         <v>56</v>
       </c>
       <c r="Q59" s="26" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="R59" s="5" t="s">
         <v>56</v>
       </c>
       <c r="S59" s="27" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="T59" s="6"/>
       <c r="U59" s="25" t="b">
@@ -10391,19 +10347,19 @@
         <v>dfu</v>
       </c>
       <c r="C60" s="20" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="D60" s="21" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="E60" s="20" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="F60" s="22" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="G60" s="20">
-        <v>10.0</v>
+        <v>16.0</v>
       </c>
       <c r="H60" s="19" t="s">
         <v>90</v>
@@ -10431,13 +10387,13 @@
         <v>56</v>
       </c>
       <c r="Q60" s="26" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="R60" s="5" t="s">
         <v>56</v>
       </c>
       <c r="S60" s="27" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="T60" s="6"/>
       <c r="U60" s="25" t="b">
@@ -10447,60 +10403,60 @@
     </row>
     <row r="61">
       <c r="A61" s="5">
-        <v>60.0</v>
+        <v>62.0</v>
       </c>
       <c r="B61" s="19" t="str">
         <f>IF(ISBLANK(A61), "", VLOOKUP(A61, Studies!A:D, 4))</f>
         <v>dfu</v>
       </c>
       <c r="C61" s="20" t="s">
-        <v>282</v>
-      </c>
-      <c r="D61" s="21" t="s">
-        <v>236</v>
+        <v>283</v>
+      </c>
+      <c r="D61" s="33" t="s">
+        <v>284</v>
       </c>
       <c r="E61" s="20" t="s">
-        <v>283</v>
+        <v>285</v>
       </c>
       <c r="F61" s="22" t="s">
-        <v>284</v>
+        <v>286</v>
       </c>
       <c r="G61" s="20">
-        <v>16.0</v>
+        <v>18.0</v>
       </c>
       <c r="H61" s="19" t="s">
-        <v>90</v>
+        <v>54</v>
       </c>
       <c r="I61" s="5" t="s">
         <v>69</v>
       </c>
       <c r="J61" s="24"/>
       <c r="K61" s="5" t="s">
-        <v>91</v>
+        <v>48</v>
       </c>
       <c r="L61" s="5" t="s">
         <v>91</v>
       </c>
       <c r="M61" s="5" t="s">
-        <v>48</v>
+        <v>91</v>
       </c>
       <c r="N61" s="5" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="O61" s="19" t="b">
         <v>0</v>
       </c>
       <c r="P61" s="5" t="s">
-        <v>56</v>
+        <v>83</v>
       </c>
       <c r="Q61" s="26" t="s">
-        <v>285</v>
+        <v>287</v>
       </c>
       <c r="R61" s="5" t="s">
-        <v>56</v>
+        <v>83</v>
       </c>
       <c r="S61" s="27" t="s">
-        <v>285</v>
+        <v>287</v>
       </c>
       <c r="T61" s="6"/>
       <c r="U61" s="25" t="b">
@@ -10510,42 +10466,44 @@
     </row>
     <row r="62">
       <c r="A62" s="5">
-        <v>62.0</v>
+        <v>65.0</v>
       </c>
       <c r="B62" s="19" t="str">
         <f>IF(ISBLANK(A62), "", VLOOKUP(A62, Studies!A:D, 4))</f>
         <v>dfu</v>
       </c>
       <c r="C62" s="20" t="s">
-        <v>286</v>
-      </c>
-      <c r="D62" s="33" t="s">
-        <v>287</v>
+        <v>288</v>
+      </c>
+      <c r="D62" s="21" t="s">
+        <v>289</v>
       </c>
       <c r="E62" s="20" t="s">
-        <v>288</v>
+        <v>290</v>
       </c>
       <c r="F62" s="22" t="s">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c r="G62" s="20">
-        <v>18.0</v>
+        <v>28.0</v>
       </c>
       <c r="H62" s="19" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="I62" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="J62" s="24"/>
+        <v>45</v>
+      </c>
+      <c r="J62" s="23" t="s">
+        <v>46</v>
+      </c>
       <c r="K62" s="5" t="s">
         <v>48</v>
       </c>
       <c r="L62" s="5" t="s">
-        <v>91</v>
+        <v>48</v>
       </c>
       <c r="M62" s="5" t="s">
-        <v>91</v>
+        <v>48</v>
       </c>
       <c r="N62" s="5" t="s">
         <v>48</v>
@@ -10554,17 +10512,15 @@
         <v>0</v>
       </c>
       <c r="P62" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="Q62" s="26" t="s">
-        <v>290</v>
+        <v>92</v>
+      </c>
+      <c r="Q62" s="31" t="s">
+        <v>292</v>
       </c>
       <c r="R62" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="S62" s="27" t="s">
-        <v>290</v>
-      </c>
+        <v>92</v>
+      </c>
+      <c r="S62" s="30"/>
       <c r="T62" s="6"/>
       <c r="U62" s="25" t="b">
         <v>0</v>
@@ -10580,19 +10536,19 @@
         <v>dfu</v>
       </c>
       <c r="C63" s="20" t="s">
+        <v>288</v>
+      </c>
+      <c r="D63" s="21" t="s">
+        <v>289</v>
+      </c>
+      <c r="E63" s="20" t="s">
+        <v>290</v>
+      </c>
+      <c r="F63" s="22" t="s">
         <v>291</v>
       </c>
-      <c r="D63" s="21" t="s">
-        <v>292</v>
-      </c>
-      <c r="E63" s="20" t="s">
-        <v>293</v>
-      </c>
-      <c r="F63" s="22" t="s">
-        <v>294</v>
-      </c>
       <c r="G63" s="20">
-        <v>28.0</v>
+        <v>16.0</v>
       </c>
       <c r="H63" s="19" t="s">
         <v>44</v>
@@ -10622,7 +10578,7 @@
         <v>92</v>
       </c>
       <c r="Q63" s="31" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="R63" s="5" t="s">
         <v>92</v>
@@ -10643,19 +10599,19 @@
         <v>dfu</v>
       </c>
       <c r="C64" s="20" t="s">
+        <v>288</v>
+      </c>
+      <c r="D64" s="21" t="s">
+        <v>289</v>
+      </c>
+      <c r="E64" s="20" t="s">
+        <v>290</v>
+      </c>
+      <c r="F64" s="22" t="s">
         <v>291</v>
       </c>
-      <c r="D64" s="21" t="s">
-        <v>292</v>
-      </c>
-      <c r="E64" s="20" t="s">
-        <v>293</v>
-      </c>
-      <c r="F64" s="22" t="s">
-        <v>294</v>
-      </c>
       <c r="G64" s="20">
-        <v>16.0</v>
+        <v>36.0</v>
       </c>
       <c r="H64" s="19" t="s">
         <v>44</v>
@@ -10685,7 +10641,7 @@
         <v>92</v>
       </c>
       <c r="Q64" s="31" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="R64" s="5" t="s">
         <v>92</v>
@@ -10706,19 +10662,19 @@
         <v>dfu</v>
       </c>
       <c r="C65" s="20" t="s">
+        <v>288</v>
+      </c>
+      <c r="D65" s="21" t="s">
+        <v>289</v>
+      </c>
+      <c r="E65" s="20" t="s">
+        <v>290</v>
+      </c>
+      <c r="F65" s="22" t="s">
         <v>291</v>
       </c>
-      <c r="D65" s="21" t="s">
-        <v>292</v>
-      </c>
-      <c r="E65" s="20" t="s">
-        <v>293</v>
-      </c>
-      <c r="F65" s="22" t="s">
-        <v>294</v>
-      </c>
       <c r="G65" s="20">
-        <v>36.0</v>
+        <v>12.0</v>
       </c>
       <c r="H65" s="19" t="s">
         <v>44</v>
@@ -10748,7 +10704,7 @@
         <v>92</v>
       </c>
       <c r="Q65" s="31" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="R65" s="5" t="s">
         <v>92</v>
@@ -10769,40 +10725,38 @@
         <v>dfu</v>
       </c>
       <c r="C66" s="20" t="s">
+        <v>288</v>
+      </c>
+      <c r="D66" s="21" t="s">
+        <v>289</v>
+      </c>
+      <c r="E66" s="20" t="s">
+        <v>290</v>
+      </c>
+      <c r="F66" s="22" t="s">
         <v>291</v>
       </c>
-      <c r="D66" s="21" t="s">
-        <v>292</v>
-      </c>
-      <c r="E66" s="20" t="s">
-        <v>293</v>
-      </c>
-      <c r="F66" s="22" t="s">
-        <v>294</v>
-      </c>
       <c r="G66" s="20">
-        <v>12.0</v>
+        <v>16.0</v>
       </c>
       <c r="H66" s="19" t="s">
-        <v>44</v>
+        <v>126</v>
       </c>
       <c r="I66" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="J66" s="23" t="s">
-        <v>46</v>
-      </c>
+        <v>69</v>
+      </c>
+      <c r="J66" s="23"/>
       <c r="K66" s="5" t="s">
-        <v>48</v>
+        <v>91</v>
       </c>
       <c r="L66" s="5" t="s">
-        <v>48</v>
+        <v>91</v>
       </c>
       <c r="M66" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="N66" s="5" t="s">
-        <v>48</v>
+        <v>91</v>
       </c>
       <c r="O66" s="19" t="b">
         <v>0</v>
@@ -10811,7 +10765,7 @@
         <v>92</v>
       </c>
       <c r="Q66" s="31" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="R66" s="5" t="s">
         <v>92</v>
@@ -10825,59 +10779,63 @@
     </row>
     <row r="67">
       <c r="A67" s="5">
-        <v>65.0</v>
+        <v>80.0</v>
       </c>
       <c r="B67" s="19" t="str">
         <f>IF(ISBLANK(A67), "", VLOOKUP(A67, Studies!A:D, 4))</f>
         <v>dfu</v>
       </c>
       <c r="C67" s="20" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
       <c r="D67" s="21" t="s">
-        <v>292</v>
+        <v>256</v>
       </c>
       <c r="E67" s="20" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="F67" s="22" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="G67" s="20">
-        <v>16.0</v>
+        <v>9.0</v>
       </c>
       <c r="H67" s="19" t="s">
-        <v>126</v>
+        <v>44</v>
       </c>
       <c r="I67" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="J67" s="23"/>
+        <v>45</v>
+      </c>
+      <c r="J67" s="23" t="s">
+        <v>82</v>
+      </c>
       <c r="K67" s="5" t="s">
-        <v>91</v>
+        <v>48</v>
       </c>
       <c r="L67" s="5" t="s">
-        <v>91</v>
+        <v>48</v>
       </c>
       <c r="M67" s="5" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="N67" s="5" t="s">
-        <v>91</v>
+        <v>48</v>
       </c>
       <c r="O67" s="19" t="b">
         <v>0</v>
       </c>
       <c r="P67" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="Q67" s="31" t="s">
-        <v>295</v>
+        <v>56</v>
+      </c>
+      <c r="Q67" s="26" t="s">
+        <v>296</v>
       </c>
       <c r="R67" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="S67" s="30"/>
+        <v>56</v>
+      </c>
+      <c r="S67" s="27" t="s">
+        <v>296</v>
+      </c>
       <c r="T67" s="6"/>
       <c r="U67" s="25" t="b">
         <v>0</v>
@@ -10886,26 +10844,26 @@
     </row>
     <row r="68">
       <c r="A68" s="5">
-        <v>80.0</v>
+        <v>112.0</v>
       </c>
       <c r="B68" s="19" t="str">
         <f>IF(ISBLANK(A68), "", VLOOKUP(A68, Studies!A:D, 4))</f>
         <v>dfu</v>
       </c>
       <c r="C68" s="20" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="D68" s="21" t="s">
-        <v>260</v>
+        <v>298</v>
       </c>
       <c r="E68" s="20" t="s">
-        <v>297</v>
+        <v>299</v>
       </c>
       <c r="F68" s="22" t="s">
-        <v>298</v>
+        <v>300</v>
       </c>
       <c r="G68" s="20">
-        <v>9.0</v>
+        <v>42.0</v>
       </c>
       <c r="H68" s="19" t="s">
         <v>44</v>
@@ -10914,10 +10872,10 @@
         <v>45</v>
       </c>
       <c r="J68" s="23" t="s">
-        <v>82</v>
+        <v>46</v>
       </c>
       <c r="K68" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="L68" s="5" t="s">
         <v>48</v>
@@ -10926,22 +10884,22 @@
         <v>48</v>
       </c>
       <c r="N68" s="5" t="s">
-        <v>48</v>
+        <v>64</v>
       </c>
       <c r="O68" s="19" t="b">
         <v>0</v>
       </c>
       <c r="P68" s="5" t="s">
-        <v>56</v>
+        <v>92</v>
       </c>
       <c r="Q68" s="26" t="s">
-        <v>299</v>
+        <v>301</v>
       </c>
       <c r="R68" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="S68" s="27" t="s">
-        <v>299</v>
+        <v>92</v>
+      </c>
+      <c r="S68" s="26" t="s">
+        <v>301</v>
       </c>
       <c r="T68" s="6"/>
       <c r="U68" s="25" t="b">
@@ -10958,10 +10916,10 @@
         <v>dfu</v>
       </c>
       <c r="C69" s="20" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="D69" s="21" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="E69" s="20" t="s">
         <v>302</v>
@@ -10970,7 +10928,7 @@
         <v>303</v>
       </c>
       <c r="G69" s="20">
-        <v>42.0</v>
+        <v>55.0</v>
       </c>
       <c r="H69" s="19" t="s">
         <v>44</v>
@@ -10994,19 +10952,19 @@
         <v>64</v>
       </c>
       <c r="O69" s="19" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P69" s="5" t="s">
         <v>92</v>
       </c>
       <c r="Q69" s="26" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="R69" s="5" t="s">
         <v>92</v>
       </c>
       <c r="S69" s="26" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="T69" s="6"/>
       <c r="U69" s="25" t="b">
@@ -11016,29 +10974,29 @@
     </row>
     <row r="70">
       <c r="A70" s="5">
-        <v>112.0</v>
+        <v>119.0</v>
       </c>
       <c r="B70" s="19" t="str">
         <f>IF(ISBLANK(A70), "", VLOOKUP(A70, Studies!A:D, 4))</f>
         <v>dfu</v>
       </c>
       <c r="C70" s="20" t="s">
-        <v>300</v>
+        <v>304</v>
       </c>
       <c r="D70" s="21" t="s">
-        <v>301</v>
+        <v>305</v>
       </c>
       <c r="E70" s="20" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="F70" s="22" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="G70" s="20">
-        <v>55.0</v>
+        <v>18.0</v>
       </c>
       <c r="H70" s="19" t="s">
-        <v>44</v>
+        <v>82</v>
       </c>
       <c r="I70" s="5" t="s">
         <v>45</v>
@@ -11047,7 +11005,7 @@
         <v>46</v>
       </c>
       <c r="K70" s="5" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="L70" s="5" t="s">
         <v>48</v>
@@ -11056,92 +11014,27 @@
         <v>48</v>
       </c>
       <c r="N70" s="5" t="s">
-        <v>64</v>
+        <v>48</v>
       </c>
       <c r="O70" s="19" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P70" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="Q70" s="26" t="s">
-        <v>304</v>
-      </c>
+        <v>49</v>
+      </c>
+      <c r="Q70" s="29"/>
       <c r="R70" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="S70" s="26" t="s">
-        <v>304</v>
-      </c>
+        <v>49</v>
+      </c>
+      <c r="S70" s="30"/>
       <c r="T70" s="6"/>
       <c r="U70" s="25" t="b">
         <v>0</v>
       </c>
       <c r="V70" s="6"/>
     </row>
-    <row r="71">
-      <c r="A71" s="5">
-        <v>119.0</v>
-      </c>
-      <c r="B71" s="19" t="str">
-        <f>IF(ISBLANK(A71), "", VLOOKUP(A71, Studies!A:D, 4))</f>
-        <v>dfu</v>
-      </c>
-      <c r="C71" s="20" t="s">
-        <v>307</v>
-      </c>
-      <c r="D71" s="21" t="s">
-        <v>308</v>
-      </c>
-      <c r="E71" s="20" t="s">
-        <v>309</v>
-      </c>
-      <c r="F71" s="22" t="s">
-        <v>310</v>
-      </c>
-      <c r="G71" s="20">
-        <v>18.0</v>
-      </c>
-      <c r="H71" s="19" t="s">
-        <v>82</v>
-      </c>
-      <c r="I71" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="J71" s="23" t="s">
-        <v>46</v>
-      </c>
-      <c r="K71" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="L71" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="M71" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="N71" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="O71" s="19" t="b">
-        <v>0</v>
-      </c>
-      <c r="P71" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="Q71" s="29"/>
-      <c r="R71" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="S71" s="30"/>
-      <c r="T71" s="6"/>
-      <c r="U71" s="25" t="b">
-        <v>0</v>
-      </c>
-      <c r="V71" s="6"/>
-    </row>
   </sheetData>
-  <autoFilter ref="$U$3:$U$71"/>
+  <autoFilter ref="$I$3:$J$70"/>
   <mergeCells count="9">
     <mergeCell ref="P2:Q2"/>
     <mergeCell ref="R2:S2"/>
@@ -11153,29 +11046,29 @@
     <mergeCell ref="E2:F2"/>
     <mergeCell ref="K2:N2"/>
   </mergeCells>
-  <conditionalFormatting sqref="U4:U71">
+  <conditionalFormatting sqref="U4:U70">
     <cfRule type="cellIs" dxfId="6" priority="1" operator="equal">
       <formula>"TRUE"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="B4:B71">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="B4:B70">
       <formula1>"dfu,jfr"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="K4:N71">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="K4:N70">
       <formula1>CategoriesAddressal!$A$2:$A$7</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="I4:I71">
-      <formula1>CategoriesMethod!$A$2:$A71</formula1>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="I4:I70">
+      <formula1>CategoriesMethod!$A$2:$A70</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="J4:J71">
-      <formula1>CategoriesTesttype!$A$2:$A71</formula1>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="J4:J70">
+      <formula1>CategoriesTesttype!$A$2:$A70</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="P4:P71 R4:R71">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="P4:P70 R4:R70">
       <formula1>"Archived,Open Source,Reachable,Upon Request,Broken,Unavailable,Private,Proprietary"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="H4:H71">
-      <formula1>CategoriesSubjects!$A$2:$A71</formula1>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="H4:H70">
+      <formula1>CategoriesSubjects!$A$2:$A70</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
@@ -11221,32 +11114,32 @@
     <hyperlink r:id="rId41" ref="S50"/>
     <hyperlink r:id="rId42" ref="Q51"/>
     <hyperlink r:id="rId43" ref="Q53"/>
-    <hyperlink r:id="rId44" ref="Q55"/>
-    <hyperlink r:id="rId45" ref="S55"/>
-    <hyperlink r:id="rId46" ref="Q56"/>
-    <hyperlink r:id="rId47" ref="S56"/>
-    <hyperlink r:id="rId48" ref="Q57"/>
-    <hyperlink r:id="rId49" ref="S57"/>
-    <hyperlink r:id="rId50" ref="Q58"/>
-    <hyperlink r:id="rId51" ref="Q59"/>
-    <hyperlink r:id="rId52" ref="S59"/>
-    <hyperlink r:id="rId53" ref="Q60"/>
-    <hyperlink r:id="rId54" ref="S60"/>
-    <hyperlink r:id="rId55" ref="Q61"/>
-    <hyperlink r:id="rId56" ref="S61"/>
-    <hyperlink r:id="rId57" ref="Q62"/>
-    <hyperlink r:id="rId58" ref="S62"/>
-    <hyperlink r:id="rId59" ref="Q63"/>
-    <hyperlink r:id="rId60" ref="Q64"/>
-    <hyperlink r:id="rId61" ref="Q65"/>
-    <hyperlink r:id="rId62" ref="Q66"/>
-    <hyperlink r:id="rId63" ref="Q67"/>
-    <hyperlink r:id="rId64" ref="Q68"/>
-    <hyperlink r:id="rId65" ref="S68"/>
-    <hyperlink r:id="rId66" ref="Q69"/>
-    <hyperlink r:id="rId67" ref="S69"/>
-    <hyperlink r:id="rId68" ref="Q70"/>
-    <hyperlink r:id="rId69" ref="S70"/>
+    <hyperlink r:id="rId44" ref="Q54"/>
+    <hyperlink r:id="rId45" ref="S54"/>
+    <hyperlink r:id="rId46" ref="Q55"/>
+    <hyperlink r:id="rId47" ref="S55"/>
+    <hyperlink r:id="rId48" ref="Q56"/>
+    <hyperlink r:id="rId49" ref="S56"/>
+    <hyperlink r:id="rId50" ref="Q57"/>
+    <hyperlink r:id="rId51" ref="Q58"/>
+    <hyperlink r:id="rId52" ref="S58"/>
+    <hyperlink r:id="rId53" ref="Q59"/>
+    <hyperlink r:id="rId54" ref="S59"/>
+    <hyperlink r:id="rId55" ref="Q60"/>
+    <hyperlink r:id="rId56" ref="S60"/>
+    <hyperlink r:id="rId57" ref="Q61"/>
+    <hyperlink r:id="rId58" ref="S61"/>
+    <hyperlink r:id="rId59" ref="Q62"/>
+    <hyperlink r:id="rId60" ref="Q63"/>
+    <hyperlink r:id="rId61" ref="Q64"/>
+    <hyperlink r:id="rId62" ref="Q65"/>
+    <hyperlink r:id="rId63" ref="Q66"/>
+    <hyperlink r:id="rId64" ref="Q67"/>
+    <hyperlink r:id="rId65" ref="S67"/>
+    <hyperlink r:id="rId66" ref="Q68"/>
+    <hyperlink r:id="rId67" ref="S68"/>
+    <hyperlink r:id="rId68" ref="Q69"/>
+    <hyperlink r:id="rId69" ref="S69"/>
   </hyperlinks>
   <drawing r:id="rId70"/>
   <legacyDrawing r:id="rId71"/>
@@ -11277,35 +11170,34 @@
     <col customWidth="1" min="8" max="8" width="16.38"/>
     <col customWidth="1" min="10" max="10" width="20.13"/>
     <col customWidth="1" min="11" max="14" width="16.38"/>
-    <col customWidth="1" min="15" max="15" width="17.63"/>
-    <col customWidth="1" min="16" max="16" width="25.13"/>
-    <col customWidth="1" min="17" max="17" width="17.63"/>
-    <col customWidth="1" min="18" max="18" width="25.13"/>
-    <col customWidth="1" min="19" max="19" width="50.13"/>
+    <col customWidth="1" min="15" max="15" width="10.13"/>
+    <col customWidth="1" min="16" max="16" width="17.63"/>
+    <col customWidth="1" min="17" max="17" width="25.13"/>
+    <col customWidth="1" min="18" max="18" width="17.63"/>
+    <col customWidth="1" min="19" max="19" width="25.13"/>
+    <col customWidth="1" min="20" max="20" width="50.13"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>18</v>
-      </c>
+      <c r="A1" s="1"/>
+      <c r="B1" s="4"/>
       <c r="C1" s="10" t="s">
         <v>9</v>
       </c>
+      <c r="F1" s="11"/>
       <c r="G1" s="10" t="s">
         <v>10</v>
       </c>
+      <c r="H1" s="11"/>
       <c r="I1" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="O1" s="12" t="s">
+      <c r="O1" s="13"/>
+      <c r="P1" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="S1" s="2" t="s">
-        <v>36</v>
-      </c>
+      <c r="S1" s="11"/>
+      <c r="T1" s="2"/>
     </row>
     <row r="2">
       <c r="A2" s="1"/>
@@ -11316,32 +11208,31 @@
       <c r="E2" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="G2" s="2" t="s">
-        <v>311</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>312</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="J2" s="14" t="s">
-        <v>26</v>
-      </c>
+      <c r="F2" s="11"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="14"/>
       <c r="K2" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="O2" s="12" t="s">
+      <c r="O2" s="13"/>
+      <c r="P2" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="Q2" s="12" t="s">
+      <c r="R2" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="S2" s="15"/>
+      <c r="S2" s="11"/>
+      <c r="T2" s="15"/>
     </row>
     <row r="3">
-      <c r="A3" s="34"/>
-      <c r="B3" s="35"/>
+      <c r="A3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>18</v>
+      </c>
       <c r="C3" s="2" t="s">
         <v>19</v>
       </c>
@@ -11354,9 +11245,18 @@
       <c r="F3" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="H3" s="35"/>
-      <c r="I3" s="34"/>
-      <c r="J3" s="36"/>
+      <c r="G3" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J3" s="14" t="s">
+        <v>26</v>
+      </c>
       <c r="K3" s="1" t="s">
         <v>27</v>
       </c>
@@ -11366,22 +11266,27 @@
       <c r="M3" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="N3" s="4" t="s">
+      <c r="N3" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="O3" s="1" t="s">
-        <v>313</v>
-      </c>
-      <c r="P3" s="17" t="s">
-        <v>314</v>
-      </c>
-      <c r="Q3" s="1" t="s">
-        <v>313</v>
-      </c>
-      <c r="R3" s="18" t="s">
-        <v>314</v>
-      </c>
-      <c r="S3" s="15"/>
+      <c r="O3" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q3" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="R3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="S3" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="T3" s="2" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="5">
@@ -11392,16 +11297,16 @@
         <v>jfr</v>
       </c>
       <c r="C4" s="20" t="s">
-        <v>315</v>
+        <v>308</v>
       </c>
       <c r="D4" s="21" t="s">
-        <v>316</v>
+        <v>309</v>
       </c>
       <c r="E4" s="20" t="s">
-        <v>317</v>
+        <v>310</v>
       </c>
       <c r="F4" s="22" t="s">
-        <v>318</v>
+        <v>311</v>
       </c>
       <c r="G4" s="20" t="s">
         <v>43</v>
@@ -11424,19 +11329,22 @@
       <c r="M4" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="N4" s="19" t="s">
-        <v>48</v>
-      </c>
-      <c r="O4" s="5" t="s">
+      <c r="N4" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="O4" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="P4" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="P4" s="29"/>
-      <c r="Q4" s="5" t="s">
+      <c r="Q4" s="29"/>
+      <c r="R4" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="R4" s="30"/>
-      <c r="S4" s="20" t="s">
-        <v>319</v>
+      <c r="S4" s="30"/>
+      <c r="T4" s="20" t="s">
+        <v>312</v>
       </c>
     </row>
     <row r="5">
@@ -11444,19 +11352,19 @@
         <v>9.0</v>
       </c>
       <c r="B5" s="19" t="s">
-        <v>320</v>
+        <v>313</v>
       </c>
       <c r="C5" s="20" t="s">
-        <v>321</v>
+        <v>314</v>
       </c>
       <c r="D5" s="21" t="s">
-        <v>322</v>
+        <v>315</v>
       </c>
       <c r="E5" s="20" t="s">
-        <v>323</v>
+        <v>316</v>
       </c>
       <c r="F5" s="22" t="s">
-        <v>324</v>
+        <v>317</v>
       </c>
       <c r="G5" s="20">
         <v>105.0</v>
@@ -11479,22 +11387,25 @@
       <c r="M5" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="N5" s="19" t="s">
+      <c r="N5" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="O5" s="5" t="s">
+      <c r="O5" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="P5" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="P5" s="26" t="s">
+      <c r="Q5" s="26" t="s">
         <v>57</v>
       </c>
-      <c r="Q5" s="5" t="s">
+      <c r="R5" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="R5" s="27" t="s">
+      <c r="S5" s="27" t="s">
         <v>57</v>
       </c>
-      <c r="S5" s="6"/>
+      <c r="T5" s="6"/>
     </row>
     <row r="6">
       <c r="A6" s="5">
@@ -11511,10 +11422,10 @@
         <v>60</v>
       </c>
       <c r="E6" s="20" t="s">
-        <v>325</v>
+        <v>318</v>
       </c>
       <c r="F6" s="22" t="s">
-        <v>326</v>
+        <v>319</v>
       </c>
       <c r="G6" s="20">
         <v>21.0</v>
@@ -11537,19 +11448,22 @@
       <c r="M6" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="N6" s="19" t="s">
+      <c r="N6" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="O6" s="5" t="s">
+      <c r="O6" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="P6" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="P6" s="29"/>
-      <c r="Q6" s="5" t="s">
+      <c r="Q6" s="29"/>
+      <c r="R6" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="R6" s="30"/>
-      <c r="S6" s="20" t="s">
-        <v>327</v>
+      <c r="S6" s="30"/>
+      <c r="T6" s="20" t="s">
+        <v>320</v>
       </c>
     </row>
     <row r="7">
@@ -11567,10 +11481,10 @@
         <v>66</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>328</v>
+        <v>321</v>
       </c>
       <c r="F7" s="19" t="s">
-        <v>329</v>
+        <v>322</v>
       </c>
       <c r="G7" s="20">
         <v>18.0</v>
@@ -11591,19 +11505,22 @@
       <c r="M7" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="N7" s="19" t="s">
+      <c r="N7" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="O7" s="5" t="s">
+      <c r="O7" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="P7" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="P7" s="29"/>
-      <c r="Q7" s="5" t="s">
+      <c r="Q7" s="29"/>
+      <c r="R7" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="R7" s="30"/>
-      <c r="S7" s="20" t="s">
-        <v>330</v>
+      <c r="S7" s="30"/>
+      <c r="T7" s="20" t="s">
+        <v>323</v>
       </c>
     </row>
     <row r="8">
@@ -11611,19 +11528,19 @@
         <v>64.0</v>
       </c>
       <c r="B8" s="19" t="s">
-        <v>320</v>
+        <v>313</v>
       </c>
       <c r="C8" s="20" t="s">
-        <v>331</v>
+        <v>324</v>
       </c>
       <c r="D8" s="21" t="s">
-        <v>332</v>
+        <v>325</v>
       </c>
       <c r="E8" s="20" t="s">
         <v>173</v>
       </c>
       <c r="F8" s="22" t="s">
-        <v>333</v>
+        <v>326</v>
       </c>
       <c r="G8" s="20">
         <v>17.0</v>
@@ -11644,20 +11561,23 @@
       <c r="M8" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="N8" s="19" t="s">
+      <c r="N8" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="O8" s="5" t="s">
+      <c r="O8" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="P8" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="P8" s="26" t="s">
+      <c r="Q8" s="26" t="s">
         <v>175</v>
       </c>
-      <c r="Q8" s="5" t="s">
+      <c r="R8" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="R8" s="30"/>
-      <c r="S8" s="6"/>
+      <c r="S8" s="30"/>
+      <c r="T8" s="6"/>
     </row>
     <row r="9">
       <c r="A9" s="5">
@@ -11671,10 +11591,10 @@
         <v>72</v>
       </c>
       <c r="D9" s="21" t="s">
-        <v>334</v>
+        <v>327</v>
       </c>
       <c r="E9" s="20" t="s">
-        <v>335</v>
+        <v>328</v>
       </c>
       <c r="F9" s="30"/>
       <c r="G9" s="20">
@@ -11698,37 +11618,40 @@
       <c r="M9" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="N9" s="19" t="s">
-        <v>48</v>
-      </c>
-      <c r="O9" s="5" t="s">
+      <c r="N9" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="O9" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="P9" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="P9" s="29"/>
-      <c r="Q9" s="5" t="s">
+      <c r="Q9" s="29"/>
+      <c r="R9" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="R9" s="30"/>
-      <c r="S9" s="6"/>
+      <c r="S9" s="30"/>
+      <c r="T9" s="6"/>
     </row>
     <row r="10">
       <c r="A10" s="5">
         <v>77.0</v>
       </c>
       <c r="B10" s="19" t="s">
-        <v>320</v>
+        <v>313</v>
       </c>
       <c r="C10" s="20" t="s">
-        <v>336</v>
+        <v>329</v>
       </c>
       <c r="D10" s="21" t="s">
-        <v>337</v>
+        <v>330</v>
       </c>
       <c r="E10" s="20" t="s">
-        <v>338</v>
+        <v>331</v>
       </c>
       <c r="F10" s="22" t="s">
-        <v>339</v>
+        <v>332</v>
       </c>
       <c r="G10" s="20">
         <v>14.0</v>
@@ -11749,39 +11672,42 @@
       <c r="M10" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="N10" s="19" t="s">
-        <v>48</v>
-      </c>
-      <c r="O10" s="5" t="s">
+      <c r="N10" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="O10" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="P10" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="P10" s="26" t="s">
+      <c r="Q10" s="26" t="s">
         <v>84</v>
       </c>
-      <c r="Q10" s="5" t="s">
+      <c r="R10" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="R10" s="30"/>
-      <c r="S10" s="6"/>
+      <c r="S10" s="30"/>
+      <c r="T10" s="6"/>
     </row>
     <row r="11">
       <c r="A11" s="5">
         <v>116.0</v>
       </c>
       <c r="B11" s="19" t="s">
-        <v>320</v>
+        <v>313</v>
       </c>
       <c r="C11" s="20" t="s">
-        <v>340</v>
+        <v>333</v>
       </c>
       <c r="D11" s="21" t="s">
-        <v>341</v>
+        <v>334</v>
       </c>
       <c r="E11" s="20" t="s">
         <v>88</v>
       </c>
       <c r="F11" s="22" t="s">
-        <v>342</v>
+        <v>335</v>
       </c>
       <c r="G11" s="20">
         <v>18.0</v>
@@ -11802,41 +11728,44 @@
       <c r="M11" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="N11" s="19" t="s">
-        <v>48</v>
-      </c>
-      <c r="O11" s="5" t="s">
+      <c r="N11" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="O11" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="P11" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="P11" s="31" t="s">
-        <v>343</v>
-      </c>
-      <c r="Q11" s="5" t="s">
+      <c r="Q11" s="31" t="s">
+        <v>336</v>
+      </c>
+      <c r="R11" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="R11" s="27" t="s">
-        <v>343</v>
-      </c>
-      <c r="S11" s="6"/>
+      <c r="S11" s="27" t="s">
+        <v>336</v>
+      </c>
+      <c r="T11" s="6"/>
     </row>
     <row r="12">
       <c r="A12" s="5">
         <v>116.0</v>
       </c>
       <c r="B12" s="19" t="s">
-        <v>320</v>
+        <v>313</v>
       </c>
       <c r="C12" s="20" t="s">
-        <v>340</v>
+        <v>333</v>
       </c>
       <c r="D12" s="21" t="s">
-        <v>341</v>
+        <v>334</v>
       </c>
       <c r="E12" s="20" t="s">
         <v>88</v>
       </c>
       <c r="F12" s="22" t="s">
-        <v>342</v>
+        <v>335</v>
       </c>
       <c r="G12" s="20">
         <v>10.0</v>
@@ -11857,41 +11786,44 @@
       <c r="M12" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="N12" s="19" t="s">
-        <v>48</v>
-      </c>
-      <c r="O12" s="5" t="s">
+      <c r="N12" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="O12" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="P12" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="P12" s="31" t="s">
-        <v>343</v>
-      </c>
-      <c r="Q12" s="5" t="s">
+      <c r="Q12" s="31" t="s">
+        <v>336</v>
+      </c>
+      <c r="R12" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="R12" s="27" t="s">
-        <v>343</v>
-      </c>
-      <c r="S12" s="6"/>
+      <c r="S12" s="27" t="s">
+        <v>336</v>
+      </c>
+      <c r="T12" s="6"/>
     </row>
     <row r="13">
       <c r="A13" s="5">
         <v>116.0</v>
       </c>
       <c r="B13" s="19" t="s">
-        <v>320</v>
+        <v>313</v>
       </c>
       <c r="C13" s="20" t="s">
-        <v>340</v>
+        <v>333</v>
       </c>
       <c r="D13" s="21" t="s">
-        <v>341</v>
+        <v>334</v>
       </c>
       <c r="E13" s="20" t="s">
         <v>88</v>
       </c>
       <c r="F13" s="22" t="s">
-        <v>342</v>
+        <v>335</v>
       </c>
       <c r="G13" s="20">
         <v>11.0</v>
@@ -11912,35 +11844,37 @@
       <c r="M13" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="N13" s="19" t="s">
-        <v>48</v>
-      </c>
-      <c r="O13" s="5" t="s">
+      <c r="N13" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="O13" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="P13" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="P13" s="31" t="s">
-        <v>343</v>
-      </c>
-      <c r="Q13" s="5" t="s">
+      <c r="Q13" s="31" t="s">
+        <v>336</v>
+      </c>
+      <c r="R13" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="R13" s="27" t="s">
-        <v>343</v>
-      </c>
-      <c r="S13" s="6"/>
+      <c r="S13" s="27" t="s">
+        <v>336</v>
+      </c>
+      <c r="T13" s="6"/>
     </row>
   </sheetData>
-  <mergeCells count="10">
-    <mergeCell ref="K2:N2"/>
-    <mergeCell ref="O2:P2"/>
+  <mergeCells count="9">
+    <mergeCell ref="P2:Q2"/>
+    <mergeCell ref="R2:S2"/>
     <mergeCell ref="C1:F1"/>
     <mergeCell ref="G1:H1"/>
     <mergeCell ref="I1:N1"/>
-    <mergeCell ref="O1:R1"/>
+    <mergeCell ref="P1:S1"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="E2:F2"/>
-    <mergeCell ref="G2:G3"/>
-    <mergeCell ref="Q2:R2"/>
+    <mergeCell ref="K2:N2"/>
   </mergeCells>
   <dataValidations>
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="K4:N13">
@@ -11955,7 +11889,7 @@
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="J4:J13">
       <formula1>CategoriesTesttype!$A$2:$A13</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="O4:O13 Q4:Q13">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="P4:P13 R4:R13">
       <formula1>"Archived,Open Source,Reachable,Upon Request,Broken,Unavailable,Private,Proprietary"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="H4:H13">
@@ -11963,16 +11897,16 @@
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="P5"/>
-    <hyperlink r:id="rId2" ref="R5"/>
-    <hyperlink r:id="rId3" ref="P8"/>
-    <hyperlink r:id="rId4" ref="P10"/>
-    <hyperlink r:id="rId5" ref="P11"/>
-    <hyperlink r:id="rId6" ref="R11"/>
-    <hyperlink r:id="rId7" ref="P12"/>
-    <hyperlink r:id="rId8" ref="R12"/>
-    <hyperlink r:id="rId9" ref="P13"/>
-    <hyperlink r:id="rId10" ref="R13"/>
+    <hyperlink r:id="rId1" ref="Q5"/>
+    <hyperlink r:id="rId2" ref="S5"/>
+    <hyperlink r:id="rId3" ref="Q8"/>
+    <hyperlink r:id="rId4" ref="Q10"/>
+    <hyperlink r:id="rId5" ref="Q11"/>
+    <hyperlink r:id="rId6" ref="S11"/>
+    <hyperlink r:id="rId7" ref="Q12"/>
+    <hyperlink r:id="rId8" ref="S12"/>
+    <hyperlink r:id="rId9" ref="Q13"/>
+    <hyperlink r:id="rId10" ref="S13"/>
   </hyperlinks>
   <drawing r:id="rId11"/>
 </worksheet>
@@ -11993,225 +11927,225 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="34" t="s">
+        <v>337</v>
+      </c>
+      <c r="B1" s="34" t="s">
+        <v>338</v>
+      </c>
+      <c r="C1" s="35" t="s">
+        <v>339</v>
+      </c>
+      <c r="F1" s="35" t="s">
+        <v>340</v>
+      </c>
+      <c r="I1" s="35" t="s">
+        <v>341</v>
+      </c>
+      <c r="L1" s="35" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="36"/>
+      <c r="B2" s="36"/>
+      <c r="C2" s="37" t="s">
+        <v>343</v>
+      </c>
+      <c r="D2" s="34" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="38" t="s">
         <v>344</v>
       </c>
-      <c r="B1" s="37" t="s">
+      <c r="F2" s="37" t="s">
+        <v>343</v>
+      </c>
+      <c r="G2" s="34" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" s="38" t="s">
+        <v>344</v>
+      </c>
+      <c r="I2" s="37" t="s">
+        <v>343</v>
+      </c>
+      <c r="J2" s="34" t="s">
+        <v>5</v>
+      </c>
+      <c r="K2" s="38" t="s">
+        <v>344</v>
+      </c>
+      <c r="L2" s="37" t="s">
+        <v>343</v>
+      </c>
+      <c r="M2" s="34" t="s">
+        <v>5</v>
+      </c>
+      <c r="N2" s="38" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="39" t="s">
         <v>345</v>
       </c>
-      <c r="C1" s="38" t="s">
+      <c r="B3" s="40" t="s">
         <v>346</v>
       </c>
-      <c r="F1" s="38" t="s">
-        <v>347</v>
-      </c>
-      <c r="I1" s="38" t="s">
-        <v>348</v>
-      </c>
-      <c r="L1" s="38" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="39"/>
-      <c r="B2" s="39"/>
-      <c r="C2" s="40" t="s">
-        <v>350</v>
-      </c>
-      <c r="D2" s="37" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" s="41" t="s">
-        <v>351</v>
-      </c>
-      <c r="F2" s="40" t="s">
-        <v>350</v>
-      </c>
-      <c r="G2" s="37" t="s">
-        <v>5</v>
-      </c>
-      <c r="H2" s="41" t="s">
-        <v>351</v>
-      </c>
-      <c r="I2" s="40" t="s">
-        <v>350</v>
-      </c>
-      <c r="J2" s="37" t="s">
-        <v>5</v>
-      </c>
-      <c r="K2" s="41" t="s">
-        <v>351</v>
-      </c>
-      <c r="L2" s="40" t="s">
-        <v>350</v>
-      </c>
-      <c r="M2" s="37" t="s">
-        <v>5</v>
-      </c>
-      <c r="N2" s="41" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="42" t="s">
-        <v>352</v>
-      </c>
-      <c r="B3" s="43" t="s">
-        <v>353</v>
-      </c>
-      <c r="C3" s="44">
+      <c r="C3" s="41">
         <f>SUMPRODUCT((Studies!D:D = A3) * (Studies!C:C = TRUE))</f>
         <v>22</v>
       </c>
-      <c r="D3" s="45">
+      <c r="D3" s="42">
         <f>SUMPRODUCT((Studies!G:G=A3) * (Studies!C:C = TRUE))</f>
         <v>4</v>
       </c>
-      <c r="E3" s="46">
+      <c r="E3" s="43">
         <f t="shared" ref="E3:E5" si="3">C3+D3</f>
         <v>26</v>
       </c>
-      <c r="F3" s="47">
+      <c r="F3" s="44">
         <f>SUMPRODUCT((Studies!D:D = A3) * (Studies!C:C = TRUE) * (Studies!E:E &gt; 0))</f>
         <v>22</v>
       </c>
-      <c r="G3" s="45">
+      <c r="G3" s="42">
         <f>SUMPRODUCT((Studies!G:G = A3) * (Studies!C:C = TRUE) * (Studies!H:H &gt; 0))</f>
         <v>4</v>
       </c>
-      <c r="H3" s="46">
+      <c r="H3" s="43">
         <f t="shared" ref="H3:H5" si="4">F3+G3</f>
         <v>26</v>
       </c>
-      <c r="I3" s="48">
+      <c r="I3" s="45">
         <f t="shared" ref="I3:K3" si="1">F3/C3</f>
         <v>1</v>
       </c>
-      <c r="J3" s="49">
+      <c r="J3" s="46">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="K3" s="50">
+      <c r="K3" s="47">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="L3" s="44">
+      <c r="L3" s="41">
         <f t="shared" ref="L3:M3" si="2">C3-F3</f>
         <v>0</v>
       </c>
-      <c r="M3" s="45">
+      <c r="M3" s="42">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="N3" s="51">
+      <c r="N3" s="48">
         <f t="shared" ref="N3:N5" si="7">L3+M3</f>
         <v>0</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="52" t="s">
-        <v>276</v>
-      </c>
-      <c r="B4" s="43" t="s">
-        <v>354</v>
-      </c>
-      <c r="C4" s="44">
+      <c r="A4" s="49" t="s">
+        <v>273</v>
+      </c>
+      <c r="B4" s="40" t="s">
+        <v>347</v>
+      </c>
+      <c r="C4" s="41">
         <f>SUMPRODUCT((Studies!D:D = A4) * (Studies!C:C = TRUE))</f>
-        <v>27</v>
-      </c>
-      <c r="D4" s="45">
+        <v>26</v>
+      </c>
+      <c r="D4" s="42">
         <f>SUMPRODUCT((Studies!G:G=A4) * (Studies!C:C = TRUE))</f>
         <v>3</v>
       </c>
-      <c r="E4" s="46">
+      <c r="E4" s="43">
         <f t="shared" si="3"/>
-        <v>30</v>
-      </c>
-      <c r="F4" s="44">
+        <v>29</v>
+      </c>
+      <c r="F4" s="41">
         <f>SUMPRODUCT((Studies!D:D = A4) * (Studies!C:C = TRUE) * (Studies!E:E &gt; 0))</f>
-        <v>27</v>
-      </c>
-      <c r="G4" s="45">
+        <v>26</v>
+      </c>
+      <c r="G4" s="42">
         <f>SUMPRODUCT((Studies!G:G = A4) * (Studies!C:C = TRUE) * (Studies!H:H &gt; 0))</f>
         <v>3</v>
       </c>
-      <c r="H4" s="46">
+      <c r="H4" s="43">
         <f t="shared" si="4"/>
-        <v>30</v>
-      </c>
-      <c r="I4" s="48">
+        <v>29</v>
+      </c>
+      <c r="I4" s="45">
         <f t="shared" ref="I4:K4" si="5">F4/C4</f>
         <v>1</v>
       </c>
-      <c r="J4" s="49">
+      <c r="J4" s="46">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
-      <c r="K4" s="50">
+      <c r="K4" s="47">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
-      <c r="L4" s="44">
+      <c r="L4" s="41">
         <f t="shared" ref="L4:M4" si="6">C4-F4</f>
         <v>0</v>
       </c>
-      <c r="M4" s="45">
+      <c r="M4" s="42">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="N4" s="51">
+      <c r="N4" s="48">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="39"/>
-      <c r="B5" s="39"/>
-      <c r="C5" s="53">
+      <c r="A5" s="36"/>
+      <c r="B5" s="36"/>
+      <c r="C5" s="50">
         <f t="shared" ref="C5:D5" si="8">SUM(C3:C4)</f>
-        <v>49</v>
-      </c>
-      <c r="D5" s="54">
+        <v>48</v>
+      </c>
+      <c r="D5" s="51">
         <f t="shared" si="8"/>
         <v>7</v>
       </c>
-      <c r="E5" s="55">
+      <c r="E5" s="52">
         <f t="shared" si="3"/>
-        <v>56</v>
-      </c>
-      <c r="F5" s="53">
+        <v>55</v>
+      </c>
+      <c r="F5" s="50">
         <f t="shared" ref="F5:G5" si="9">SUM(F3:F4)</f>
-        <v>49</v>
-      </c>
-      <c r="G5" s="54">
+        <v>48</v>
+      </c>
+      <c r="G5" s="51">
         <f t="shared" si="9"/>
         <v>7</v>
       </c>
-      <c r="H5" s="55">
+      <c r="H5" s="52">
         <f t="shared" si="4"/>
-        <v>56</v>
-      </c>
-      <c r="I5" s="56">
+        <v>55</v>
+      </c>
+      <c r="I5" s="53">
         <f t="shared" ref="I5:M5" si="10">SUM(I3:I4)</f>
         <v>2</v>
       </c>
-      <c r="J5" s="57">
+      <c r="J5" s="54">
         <f t="shared" si="10"/>
         <v>2</v>
       </c>
-      <c r="K5" s="58">
+      <c r="K5" s="55">
         <f t="shared" si="10"/>
         <v>2</v>
       </c>
-      <c r="L5" s="53">
+      <c r="L5" s="50">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="M5" s="54">
+      <c r="M5" s="51">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="N5" s="55">
+      <c r="N5" s="52">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -12292,21 +12226,21 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="2" t="s">
-        <v>312</v>
-      </c>
-      <c r="B1" s="59" t="s">
-        <v>355</v>
-      </c>
-      <c r="C1" s="60" t="s">
-        <v>356</v>
+        <v>348</v>
+      </c>
+      <c r="B1" s="56" t="s">
+        <v>349</v>
+      </c>
+      <c r="C1" s="57" t="s">
+        <v>350</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="61" t="s">
+      <c r="A2" s="58" t="s">
         <v>44</v>
       </c>
       <c r="B2" s="20" t="s">
-        <v>357</v>
+        <v>351</v>
       </c>
       <c r="C2" s="8">
         <f>COUNTIF(Extraction!H:H, A2)</f>
@@ -12314,11 +12248,11 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="61" t="s">
+      <c r="A3" s="58" t="s">
         <v>90</v>
       </c>
       <c r="B3" s="20" t="s">
-        <v>358</v>
+        <v>352</v>
       </c>
       <c r="C3" s="8">
         <f>COUNTIF(Extraction!H:H, A3)</f>
@@ -12326,11 +12260,11 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="61" t="s">
+      <c r="A4" s="58" t="s">
         <v>126</v>
       </c>
       <c r="B4" s="20" t="s">
-        <v>359</v>
+        <v>353</v>
       </c>
       <c r="C4" s="8">
         <f>COUNTIF(Extraction!H:H, A4)</f>
@@ -12338,11 +12272,11 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="61" t="s">
-        <v>360</v>
+      <c r="A5" s="58" t="s">
+        <v>354</v>
       </c>
       <c r="B5" s="20" t="s">
-        <v>361</v>
+        <v>355</v>
       </c>
       <c r="C5" s="8">
         <f>COUNTIF(Extraction!H:H, A5)</f>
@@ -12350,11 +12284,11 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="61" t="s">
-        <v>205</v>
+      <c r="A6" s="58" t="s">
+        <v>206</v>
       </c>
       <c r="B6" s="20" t="s">
-        <v>362</v>
+        <v>356</v>
       </c>
       <c r="C6" s="8">
         <f>COUNTIF(Extraction!H:H, A6)</f>
@@ -12362,23 +12296,23 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="61" t="s">
+      <c r="A7" s="58" t="s">
         <v>54</v>
       </c>
       <c r="B7" s="20" t="s">
-        <v>363</v>
+        <v>357</v>
       </c>
       <c r="C7" s="8">
         <f>COUNTIF(Extraction!H:H, A7)</f>
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="61" t="s">
+      <c r="A8" s="58" t="s">
         <v>81</v>
       </c>
       <c r="B8" s="20" t="s">
-        <v>364</v>
+        <v>358</v>
       </c>
       <c r="C8" s="8">
         <f>COUNTIF(Extraction!H:H, A8)</f>
@@ -12386,11 +12320,11 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="61" t="s">
-        <v>200</v>
+      <c r="A9" s="58" t="s">
+        <v>201</v>
       </c>
       <c r="B9" s="20" t="s">
-        <v>365</v>
+        <v>359</v>
       </c>
       <c r="C9" s="8">
         <f>COUNTIF(Extraction!H:H, A9)</f>
@@ -12398,11 +12332,11 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="61" t="s">
+      <c r="A10" s="58" t="s">
         <v>82</v>
       </c>
       <c r="B10" s="20" t="s">
-        <v>366</v>
+        <v>360</v>
       </c>
       <c r="C10" s="8">
         <f>COUNTIF(Extraction!H:H, A10)</f>
@@ -12442,43 +12376,43 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="60" t="s">
-        <v>367</v>
-      </c>
-      <c r="B1" s="60" t="s">
+      <c r="A1" s="57" t="s">
+        <v>361</v>
+      </c>
+      <c r="B1" s="57" t="s">
         <v>25</v>
       </c>
-      <c r="C1" s="59" t="s">
-        <v>355</v>
-      </c>
-      <c r="D1" s="60" t="s">
-        <v>356</v>
+      <c r="C1" s="56" t="s">
+        <v>349</v>
+      </c>
+      <c r="D1" s="57" t="s">
+        <v>350</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="62" t="s">
+      <c r="A2" s="59" t="s">
         <v>45</v>
       </c>
-      <c r="B2" s="63" t="s">
-        <v>368</v>
-      </c>
-      <c r="C2" s="64" t="s">
-        <v>369</v>
+      <c r="B2" s="60" t="s">
+        <v>362</v>
+      </c>
+      <c r="C2" s="61" t="s">
+        <v>363</v>
       </c>
       <c r="D2" s="8">
         <f>COUNTIF(Extraction!I:I, A2)</f>
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="62" t="s">
-        <v>370</v>
-      </c>
-      <c r="B3" s="63" t="s">
-        <v>371</v>
-      </c>
-      <c r="C3" s="64" t="s">
-        <v>372</v>
+      <c r="A3" s="59" t="s">
+        <v>364</v>
+      </c>
+      <c r="B3" s="60" t="s">
+        <v>365</v>
+      </c>
+      <c r="C3" s="61" t="s">
+        <v>366</v>
       </c>
       <c r="D3" s="8">
         <f>COUNTIF(Extraction!I:I, A3)</f>
@@ -12486,14 +12420,14 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="62" t="s">
+      <c r="A4" s="59" t="s">
         <v>69</v>
       </c>
-      <c r="B4" s="63" t="s">
-        <v>373</v>
-      </c>
-      <c r="C4" s="64" t="s">
-        <v>374</v>
+      <c r="B4" s="60" t="s">
+        <v>367</v>
+      </c>
+      <c r="C4" s="61" t="s">
+        <v>368</v>
       </c>
       <c r="D4" s="8">
         <f>COUNTIF(Extraction!I:I, A4)</f>
@@ -12501,14 +12435,14 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="62" t="s">
-        <v>375</v>
-      </c>
-      <c r="B5" s="63" t="s">
-        <v>376</v>
-      </c>
-      <c r="C5" s="64" t="s">
-        <v>377</v>
+      <c r="A5" s="59" t="s">
+        <v>369</v>
+      </c>
+      <c r="B5" s="60" t="s">
+        <v>370</v>
+      </c>
+      <c r="C5" s="61" t="s">
+        <v>371</v>
       </c>
       <c r="D5" s="8">
         <f>COUNTIF(Extraction!I:I, A5)</f>
@@ -12516,12 +12450,12 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="62" t="s">
+      <c r="A6" s="59" t="s">
         <v>82</v>
       </c>
       <c r="B6" s="5"/>
       <c r="C6" s="20" t="s">
-        <v>378</v>
+        <v>372</v>
       </c>
       <c r="D6" s="8">
         <f>COUNTIF(Extraction!I:I, A6)</f>
@@ -12529,12 +12463,12 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="65" t="s">
+      <c r="A7" s="62" t="s">
         <v>81</v>
       </c>
       <c r="B7" s="5"/>
       <c r="C7" s="20" t="s">
-        <v>379</v>
+        <v>373</v>
       </c>
       <c r="D7" s="8">
         <f>COUNTIF(Extraction!I:I, A7)</f>
@@ -12574,22 +12508,22 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="60" t="s">
-        <v>367</v>
-      </c>
-      <c r="B1" s="59" t="s">
-        <v>355</v>
-      </c>
-      <c r="C1" s="60" t="s">
-        <v>356</v>
+      <c r="A1" s="57" t="s">
+        <v>361</v>
+      </c>
+      <c r="B1" s="56" t="s">
+        <v>349</v>
+      </c>
+      <c r="C1" s="57" t="s">
+        <v>350</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="65" t="s">
-        <v>380</v>
+      <c r="A2" s="62" t="s">
+        <v>374</v>
       </c>
       <c r="B2" s="20" t="s">
-        <v>381</v>
+        <v>375</v>
       </c>
       <c r="C2" s="8">
         <f>COUNTIF(Extraction!J:J, A2)</f>
@@ -12597,11 +12531,11 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="65" t="s">
+      <c r="A3" s="62" t="s">
         <v>108</v>
       </c>
       <c r="B3" s="20" t="s">
-        <v>382</v>
+        <v>376</v>
       </c>
       <c r="C3" s="8">
         <f>COUNTIF(Extraction!J:J, A3)</f>
@@ -12609,11 +12543,11 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="65" t="s">
+      <c r="A4" s="62" t="s">
         <v>46</v>
       </c>
       <c r="B4" s="20" t="s">
-        <v>383</v>
+        <v>377</v>
       </c>
       <c r="C4" s="8">
         <f>COUNTIF(Extraction!J:J, A4)</f>
@@ -12621,11 +12555,11 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="65" t="s">
+      <c r="A5" s="62" t="s">
         <v>76</v>
       </c>
       <c r="B5" s="20" t="s">
-        <v>384</v>
+        <v>378</v>
       </c>
       <c r="C5" s="8">
         <f>COUNTIF(Extraction!J:J, A5)</f>
@@ -12633,43 +12567,55 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="65" t="s">
+      <c r="A6" s="62" t="s">
         <v>183</v>
       </c>
       <c r="B6" s="20" t="s">
-        <v>385</v>
+        <v>379</v>
       </c>
       <c r="C6" s="8">
         <f>COUNTIF(Extraction!J:J, A6)</f>
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="65" t="s">
-        <v>63</v>
+      <c r="A7" s="62" t="s">
+        <v>194</v>
       </c>
       <c r="B7" s="20" t="s">
-        <v>386</v>
+        <v>380</v>
       </c>
       <c r="C7" s="8">
         <f>COUNTIF(Extraction!J:J, A7)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="65" t="s">
-        <v>82</v>
+      <c r="A8" s="62" t="s">
+        <v>63</v>
       </c>
       <c r="B8" s="20" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
       <c r="C8" s="8">
         <f>COUNTIF(Extraction!J:J, A8)</f>
         <v>1</v>
       </c>
     </row>
+    <row r="9">
+      <c r="A9" s="62" t="s">
+        <v>82</v>
+      </c>
+      <c r="B9" s="20" t="s">
+        <v>382</v>
+      </c>
+      <c r="C9" s="8">
+        <f>COUNTIF(Extraction!J:J, A9)</f>
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="C2:C8">
+  <conditionalFormatting sqref="C2:C9">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
@@ -12701,11 +12647,11 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="60" t="s">
-        <v>367</v>
-      </c>
-      <c r="B1" s="59" t="s">
-        <v>355</v>
+      <c r="A1" s="57" t="s">
+        <v>361</v>
+      </c>
+      <c r="B1" s="56" t="s">
+        <v>349</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>27</v>
@@ -12714,18 +12660,18 @@
         <v>28</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>388</v>
+        <v>383</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="66" t="s">
+      <c r="A2" s="63" t="s">
         <v>91</v>
       </c>
       <c r="B2" s="20" t="s">
-        <v>389</v>
+        <v>384</v>
       </c>
       <c r="C2" s="8">
         <f>COUNTIF(Extraction!K:K, $A2)</f>
@@ -12737,19 +12683,19 @@
       </c>
       <c r="E2" s="8">
         <f>COUNTIF(Extraction!M:M, $A2)</f>
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F2" s="8">
         <f>COUNTIF(Extraction!N:N, $A2)</f>
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="67" t="s">
-        <v>390</v>
+      <c r="A3" s="64" t="s">
+        <v>385</v>
       </c>
       <c r="B3" s="20" t="s">
-        <v>391</v>
+        <v>386</v>
       </c>
       <c r="C3" s="8">
         <f>COUNTIF(Extraction!K:K, $A3)</f>
@@ -12769,11 +12715,11 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="68" t="s">
+      <c r="A4" s="65" t="s">
         <v>64</v>
       </c>
       <c r="B4" s="20" t="s">
-        <v>392</v>
+        <v>387</v>
       </c>
       <c r="C4" s="8">
         <f>COUNTIF(Extraction!K:K, $A4)</f>
@@ -12781,27 +12727,27 @@
       </c>
       <c r="D4" s="8">
         <f>COUNTIF(Extraction!L:L, $A4)</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E4" s="8">
         <f>COUNTIF(Extraction!M:M, $A4)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F4" s="8">
         <f>COUNTIF(Extraction!N:N, $A4)</f>
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="69" t="s">
+      <c r="A5" s="66" t="s">
         <v>47</v>
       </c>
       <c r="B5" s="20" t="s">
-        <v>393</v>
+        <v>388</v>
       </c>
       <c r="C5" s="8">
         <f>COUNTIF(Extraction!K:K, $A5)</f>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D5" s="8">
         <f>COUNTIF(Extraction!L:L, $A5)</f>
@@ -12809,19 +12755,19 @@
       </c>
       <c r="E5" s="8">
         <f>COUNTIF(Extraction!M:M, $A5)</f>
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F5" s="8">
         <f>COUNTIF(Extraction!N:N, $A5)</f>
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="70" t="s">
+      <c r="A6" s="67" t="s">
         <v>55</v>
       </c>
       <c r="B6" s="20" t="s">
-        <v>394</v>
+        <v>389</v>
       </c>
       <c r="C6" s="8">
         <f>COUNTIF(Extraction!K:K, $A6)</f>
@@ -12833,7 +12779,7 @@
       </c>
       <c r="E6" s="8">
         <f>COUNTIF(Extraction!M:M, $A6)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F6" s="8">
         <f>COUNTIF(Extraction!N:N, $A6)</f>
@@ -12841,11 +12787,11 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="71" t="s">
+      <c r="A7" s="68" t="s">
         <v>48</v>
       </c>
       <c r="B7" s="20" t="s">
-        <v>395</v>
+        <v>390</v>
       </c>
       <c r="C7" s="8">
         <f>COUNTIF(Extraction!K:K, $A7)</f>
@@ -12857,7 +12803,7 @@
       </c>
       <c r="E7" s="8">
         <f>COUNTIF(Extraction!M:M, $A7)</f>
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F7" s="8">
         <f>COUNTIF(Extraction!N:N, $A7)</f>

</xml_diff>